<commit_message>
auth orders supplier 요구사항 반영 완료
</commit_message>
<xml_diff>
--- a/ERP/public/data/template.xlsx
+++ b/ERP/public/data/template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewLocalUser\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NewLocalUser\Desktop\NEXT\crimson\Crimson-ERP-FE\ERP\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67DA7A68-1CA8-4F64-8EAC-8D9EAF6A1EC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DBF80EE-9CD1-4F38-8480-2F9F497885BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="10965" windowHeight="12863" xr2:uid="{6EBF5798-06D6-634B-B56A-75BC59B54246}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{6EBF5798-06D6-634B-B56A-75BC59B54246}"/>
   </bookViews>
   <sheets>
     <sheet name="(주)고대미래발주서" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="51">
   <si>
     <t>사업자번호</t>
   </si>
@@ -126,26 +126,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>팩토리코퍼레이션</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> 010-6675-7797</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>박한솔</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>이메일</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>hspark_factcorp@kakao.com</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>아래와 같이 발주하오니 기일 내 필히 납품하여 주시기 바랍니다.</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -154,18 +138,10 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>납품일자 : 샘플 컨펌후 진행으로 2월초 예상</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>납품장소 :</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>고려대학교100주년기념관(크림슨스토어)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>구매비용 :</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -182,10 +158,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>2,013,000 )</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>)</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -234,24 +206,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>노트북파우치 샘플
-(15인치, 자수)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>38.5*28</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>cm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>노트북파우치 본제품
-(15인치, 자수)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>합               계</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -280,12 +234,6 @@
   </si>
   <si>
     <t>메 일</t>
-  </si>
-  <si>
-    <t>김재형</t>
-  </si>
-  <si>
-    <t>이백일만삼천</t>
   </si>
   <si>
     <t>· 샘플 제작, 컨펌후 제작 총액 100% 2,013,000원 (VAT포함) 세금계산서 선발행, 
@@ -1031,6 +979,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1040,10 +1009,301 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1109,320 +1369,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="40" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2165,8 +2113,8 @@
   </sheetPr>
   <dimension ref="A2:AF34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AX10" sqref="AX10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.3515625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2188,111 +2136,111 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="35"/>
-      <c r="B2" s="35"/>
-      <c r="C2" s="35"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="Q2" s="23" t="s">
+      <c r="A2" s="139"/>
+      <c r="B2" s="139"/>
+      <c r="C2" s="139"/>
+      <c r="D2" s="124"/>
+      <c r="E2" s="124"/>
+      <c r="F2" s="124"/>
+      <c r="G2" s="124"/>
+      <c r="H2" s="124"/>
+      <c r="I2" s="124"/>
+      <c r="J2" s="124"/>
+      <c r="K2" s="124"/>
+      <c r="L2" s="124"/>
+      <c r="M2" s="124"/>
+      <c r="N2" s="124"/>
+      <c r="O2" s="124"/>
+      <c r="Q2" s="127" t="s">
         <v>0</v>
       </c>
-      <c r="R2" s="24"/>
-      <c r="S2" s="24"/>
-      <c r="T2" s="24"/>
-      <c r="U2" s="25" t="s">
+      <c r="R2" s="128"/>
+      <c r="S2" s="128"/>
+      <c r="T2" s="128"/>
+      <c r="U2" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="27"/>
+      <c r="V2" s="130"/>
+      <c r="W2" s="130"/>
+      <c r="X2" s="130"/>
+      <c r="Y2" s="130"/>
+      <c r="Z2" s="130"/>
+      <c r="AA2" s="130"/>
+      <c r="AB2" s="130"/>
+      <c r="AC2" s="130"/>
+      <c r="AD2" s="130"/>
+      <c r="AE2" s="130"/>
+      <c r="AF2" s="131"/>
     </row>
     <row r="3" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="35"/>
-      <c r="B3" s="35"/>
-      <c r="C3" s="35"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
-      <c r="N3" s="20"/>
-      <c r="O3" s="20"/>
-      <c r="Q3" s="21" t="s">
+      <c r="A3" s="139"/>
+      <c r="B3" s="139"/>
+      <c r="C3" s="139"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
+      <c r="K3" s="124"/>
+      <c r="L3" s="124"/>
+      <c r="M3" s="124"/>
+      <c r="N3" s="124"/>
+      <c r="O3" s="124"/>
+      <c r="Q3" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="R3" s="22"/>
-      <c r="S3" s="22"/>
-      <c r="T3" s="22"/>
-      <c r="U3" s="28" t="s">
+      <c r="R3" s="126"/>
+      <c r="S3" s="126"/>
+      <c r="T3" s="126"/>
+      <c r="U3" s="132" t="s">
         <v>3</v>
       </c>
-      <c r="V3" s="29"/>
-      <c r="W3" s="29"/>
-      <c r="X3" s="29"/>
-      <c r="Y3" s="29"/>
-      <c r="Z3" s="29"/>
-      <c r="AA3" s="29"/>
-      <c r="AB3" s="29"/>
-      <c r="AC3" s="29"/>
-      <c r="AD3" s="29"/>
-      <c r="AE3" s="29"/>
-      <c r="AF3" s="30"/>
+      <c r="V3" s="133"/>
+      <c r="W3" s="133"/>
+      <c r="X3" s="133"/>
+      <c r="Y3" s="133"/>
+      <c r="Z3" s="133"/>
+      <c r="AA3" s="133"/>
+      <c r="AB3" s="133"/>
+      <c r="AC3" s="133"/>
+      <c r="AD3" s="133"/>
+      <c r="AE3" s="133"/>
+      <c r="AF3" s="134"/>
     </row>
     <row r="4" spans="1:32" ht="66" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="Q4" s="21" t="s">
-        <v>59</v>
-      </c>
-      <c r="R4" s="22"/>
-      <c r="S4" s="22"/>
-      <c r="T4" s="22"/>
-      <c r="U4" s="31" t="s">
+      <c r="Q4" s="125" t="s">
+        <v>48</v>
+      </c>
+      <c r="R4" s="126"/>
+      <c r="S4" s="126"/>
+      <c r="T4" s="126"/>
+      <c r="U4" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="V4" s="32"/>
-      <c r="W4" s="32"/>
-      <c r="X4" s="32"/>
-      <c r="Y4" s="32"/>
-      <c r="Z4" s="32"/>
-      <c r="AA4" s="32"/>
-      <c r="AB4" s="32"/>
-      <c r="AC4" s="32"/>
-      <c r="AD4" s="32"/>
-      <c r="AE4" s="32"/>
-      <c r="AF4" s="33"/>
+      <c r="V4" s="136"/>
+      <c r="W4" s="136"/>
+      <c r="X4" s="136"/>
+      <c r="Y4" s="136"/>
+      <c r="Z4" s="136"/>
+      <c r="AA4" s="136"/>
+      <c r="AB4" s="136"/>
+      <c r="AC4" s="136"/>
+      <c r="AD4" s="136"/>
+      <c r="AE4" s="136"/>
+      <c r="AF4" s="137"/>
     </row>
     <row r="5" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="34"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
-      <c r="G5" s="34"/>
-      <c r="H5" s="34"/>
-      <c r="I5" s="34"/>
+      <c r="A5" s="138"/>
+      <c r="B5" s="138"/>
+      <c r="C5" s="138"/>
+      <c r="D5" s="138"/>
+      <c r="E5" s="138"/>
+      <c r="F5" s="138"/>
+      <c r="G5" s="138"/>
+      <c r="H5" s="138"/>
+      <c r="I5" s="138"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -2300,108 +2248,108 @@
       <c r="N5" s="2"/>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="21" t="s">
+      <c r="Q5" s="125" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="22"/>
-      <c r="S5" s="22"/>
-      <c r="T5" s="22"/>
-      <c r="U5" s="28" t="s">
+      <c r="R5" s="126"/>
+      <c r="S5" s="126"/>
+      <c r="T5" s="126"/>
+      <c r="U5" s="132" t="s">
         <v>6</v>
       </c>
-      <c r="V5" s="29"/>
-      <c r="W5" s="29"/>
-      <c r="X5" s="29"/>
-      <c r="Y5" s="29"/>
-      <c r="Z5" s="29"/>
-      <c r="AA5" s="29"/>
-      <c r="AB5" s="29"/>
-      <c r="AC5" s="29"/>
-      <c r="AD5" s="29"/>
-      <c r="AE5" s="29"/>
-      <c r="AF5" s="30"/>
+      <c r="V5" s="133"/>
+      <c r="W5" s="133"/>
+      <c r="X5" s="133"/>
+      <c r="Y5" s="133"/>
+      <c r="Z5" s="133"/>
+      <c r="AA5" s="133"/>
+      <c r="AB5" s="133"/>
+      <c r="AC5" s="133"/>
+      <c r="AD5" s="133"/>
+      <c r="AE5" s="133"/>
+      <c r="AF5" s="134"/>
     </row>
     <row r="6" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="36" t="s">
+      <c r="A6" s="140" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="36"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="36"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36"/>
-      <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
-      <c r="N6" s="36"/>
-      <c r="O6" s="36"/>
+      <c r="B6" s="140"/>
+      <c r="C6" s="140"/>
+      <c r="D6" s="140"/>
+      <c r="E6" s="140"/>
+      <c r="F6" s="140"/>
+      <c r="G6" s="140"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="140"/>
+      <c r="J6" s="140"/>
+      <c r="K6" s="140"/>
+      <c r="L6" s="140"/>
+      <c r="M6" s="140"/>
+      <c r="N6" s="140"/>
+      <c r="O6" s="140"/>
       <c r="P6" s="8"/>
-      <c r="Q6" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="R6" s="22"/>
-      <c r="S6" s="22"/>
-      <c r="T6" s="22"/>
-      <c r="U6" s="37" t="s">
+      <c r="Q6" s="125" t="s">
+        <v>49</v>
+      </c>
+      <c r="R6" s="126"/>
+      <c r="S6" s="126"/>
+      <c r="T6" s="126"/>
+      <c r="U6" s="141" t="s">
         <v>8</v>
       </c>
-      <c r="V6" s="29"/>
-      <c r="W6" s="29"/>
-      <c r="X6" s="29"/>
-      <c r="Y6" s="29"/>
-      <c r="Z6" s="29"/>
-      <c r="AA6" s="29"/>
-      <c r="AB6" s="29"/>
-      <c r="AC6" s="29"/>
-      <c r="AD6" s="29"/>
-      <c r="AE6" s="29"/>
-      <c r="AF6" s="30"/>
+      <c r="V6" s="133"/>
+      <c r="W6" s="133"/>
+      <c r="X6" s="133"/>
+      <c r="Y6" s="133"/>
+      <c r="Z6" s="133"/>
+      <c r="AA6" s="133"/>
+      <c r="AB6" s="133"/>
+      <c r="AC6" s="133"/>
+      <c r="AD6" s="133"/>
+      <c r="AE6" s="133"/>
+      <c r="AF6" s="134"/>
     </row>
     <row r="7" spans="1:32" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="36"/>
-      <c r="B7" s="36"/>
-      <c r="C7" s="36"/>
-      <c r="D7" s="36"/>
-      <c r="E7" s="36"/>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36"/>
-      <c r="H7" s="36"/>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
-      <c r="K7" s="36"/>
-      <c r="L7" s="36"/>
-      <c r="M7" s="36"/>
-      <c r="N7" s="36"/>
-      <c r="O7" s="36"/>
+      <c r="A7" s="140"/>
+      <c r="B7" s="140"/>
+      <c r="C7" s="140"/>
+      <c r="D7" s="140"/>
+      <c r="E7" s="140"/>
+      <c r="F7" s="140"/>
+      <c r="G7" s="140"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="140"/>
+      <c r="J7" s="140"/>
+      <c r="K7" s="140"/>
+      <c r="L7" s="140"/>
+      <c r="M7" s="140"/>
+      <c r="N7" s="140"/>
+      <c r="O7" s="140"/>
       <c r="P7" s="8"/>
-      <c r="Q7" s="38" t="s">
+      <c r="Q7" s="142" t="s">
         <v>9</v>
       </c>
-      <c r="R7" s="39"/>
-      <c r="S7" s="39"/>
-      <c r="T7" s="39"/>
-      <c r="U7" s="40" t="s">
+      <c r="R7" s="143"/>
+      <c r="S7" s="143"/>
+      <c r="T7" s="143"/>
+      <c r="U7" s="144" t="s">
         <v>10</v>
       </c>
-      <c r="V7" s="41"/>
-      <c r="W7" s="41"/>
-      <c r="X7" s="41"/>
-      <c r="Y7" s="41"/>
-      <c r="Z7" s="41" t="s">
+      <c r="V7" s="91"/>
+      <c r="W7" s="91"/>
+      <c r="X7" s="91"/>
+      <c r="Y7" s="91"/>
+      <c r="Z7" s="91" t="s">
         <v>11</v>
       </c>
-      <c r="AA7" s="41"/>
-      <c r="AB7" s="41" t="s">
+      <c r="AA7" s="91"/>
+      <c r="AB7" s="91" t="s">
         <v>12</v>
       </c>
-      <c r="AC7" s="41"/>
-      <c r="AD7" s="41"/>
-      <c r="AE7" s="41"/>
-      <c r="AF7" s="46"/>
+      <c r="AC7" s="91"/>
+      <c r="AD7" s="91"/>
+      <c r="AE7" s="91"/>
+      <c r="AF7" s="92"/>
     </row>
     <row r="8" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
@@ -2438,740 +2386,696 @@
       <c r="AF8" s="2"/>
     </row>
     <row r="9" spans="1:32" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="95" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="55" t="s">
+      <c r="B9" s="96"/>
+      <c r="C9" s="96"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="101" t="s">
         <v>14</v>
       </c>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="57" t="s">
+      <c r="F9" s="102"/>
+      <c r="G9" s="102"/>
+      <c r="H9" s="102"/>
+      <c r="I9" s="81" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="57"/>
-      <c r="K9" s="57"/>
-      <c r="L9" s="57"/>
-      <c r="M9" s="57"/>
-      <c r="N9" s="57"/>
-      <c r="O9" s="57"/>
-      <c r="P9" s="57"/>
-      <c r="Q9" s="57"/>
-      <c r="R9" s="57"/>
-      <c r="S9" s="56" t="s">
+      <c r="J9" s="81"/>
+      <c r="K9" s="81"/>
+      <c r="L9" s="81"/>
+      <c r="M9" s="81"/>
+      <c r="N9" s="81"/>
+      <c r="O9" s="81"/>
+      <c r="P9" s="81"/>
+      <c r="Q9" s="81"/>
+      <c r="R9" s="81"/>
+      <c r="S9" s="102" t="s">
         <v>16</v>
       </c>
-      <c r="T9" s="56"/>
-      <c r="U9" s="56"/>
-      <c r="V9" s="56"/>
-      <c r="W9" s="58" t="s">
+      <c r="T9" s="102"/>
+      <c r="U9" s="102"/>
+      <c r="V9" s="102"/>
+      <c r="W9" s="103" t="s">
         <v>17</v>
       </c>
-      <c r="X9" s="58"/>
-      <c r="Y9" s="58"/>
-      <c r="Z9" s="58"/>
-      <c r="AA9" s="58"/>
-      <c r="AB9" s="58"/>
-      <c r="AC9" s="58"/>
-      <c r="AD9" s="58"/>
-      <c r="AE9" s="58"/>
-      <c r="AF9" s="59"/>
+      <c r="X9" s="103"/>
+      <c r="Y9" s="103"/>
+      <c r="Z9" s="103"/>
+      <c r="AA9" s="103"/>
+      <c r="AB9" s="103"/>
+      <c r="AC9" s="103"/>
+      <c r="AD9" s="103"/>
+      <c r="AE9" s="103"/>
+      <c r="AF9" s="104"/>
     </row>
     <row r="10" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="52"/>
-      <c r="B10" s="53"/>
-      <c r="C10" s="53"/>
-      <c r="D10" s="54"/>
-      <c r="E10" s="69" t="s">
+      <c r="A10" s="98"/>
+      <c r="B10" s="99"/>
+      <c r="C10" s="99"/>
+      <c r="D10" s="100"/>
+      <c r="E10" s="114" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="70"/>
-      <c r="G10" s="70"/>
-      <c r="H10" s="70"/>
-      <c r="I10" s="71" t="s">
-        <v>61</v>
-      </c>
-      <c r="J10" s="71"/>
-      <c r="K10" s="71"/>
-      <c r="L10" s="71"/>
-      <c r="M10" s="71"/>
-      <c r="N10" s="71"/>
-      <c r="O10" s="71"/>
-      <c r="P10" s="71"/>
-      <c r="Q10" s="71"/>
-      <c r="R10" s="71"/>
-      <c r="S10" s="70" t="s">
+      <c r="F10" s="115"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="115"/>
+      <c r="I10" s="116"/>
+      <c r="J10" s="116"/>
+      <c r="K10" s="116"/>
+      <c r="L10" s="116"/>
+      <c r="M10" s="116"/>
+      <c r="N10" s="116"/>
+      <c r="O10" s="116"/>
+      <c r="P10" s="116"/>
+      <c r="Q10" s="116"/>
+      <c r="R10" s="116"/>
+      <c r="S10" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="T10" s="70"/>
-      <c r="U10" s="70"/>
-      <c r="V10" s="70"/>
-      <c r="W10" s="47" t="s">
+      <c r="T10" s="115"/>
+      <c r="U10" s="115"/>
+      <c r="V10" s="115"/>
+      <c r="W10" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="X10" s="47"/>
-      <c r="Y10" s="47"/>
-      <c r="Z10" s="47"/>
-      <c r="AA10" s="47"/>
-      <c r="AB10" s="47"/>
-      <c r="AC10" s="47"/>
-      <c r="AD10" s="47"/>
-      <c r="AE10" s="47"/>
-      <c r="AF10" s="48"/>
+      <c r="X10" s="93"/>
+      <c r="Y10" s="93"/>
+      <c r="Z10" s="93"/>
+      <c r="AA10" s="93"/>
+      <c r="AB10" s="93"/>
+      <c r="AC10" s="93"/>
+      <c r="AD10" s="93"/>
+      <c r="AE10" s="93"/>
+      <c r="AF10" s="94"/>
     </row>
     <row r="11" spans="1:32" ht="19.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="105" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="66" t="s">
+      <c r="B11" s="106"/>
+      <c r="C11" s="106"/>
+      <c r="D11" s="107"/>
+      <c r="E11" s="111" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="67"/>
-      <c r="G11" s="67"/>
-      <c r="H11" s="67"/>
-      <c r="I11" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="J11" s="68"/>
-      <c r="K11" s="68"/>
-      <c r="L11" s="68"/>
-      <c r="M11" s="68"/>
-      <c r="N11" s="68"/>
-      <c r="O11" s="68"/>
-      <c r="P11" s="68"/>
-      <c r="Q11" s="68"/>
-      <c r="R11" s="68"/>
-      <c r="S11" s="67" t="s">
+      <c r="F11" s="112"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="112"/>
+      <c r="I11" s="113"/>
+      <c r="J11" s="113"/>
+      <c r="K11" s="113"/>
+      <c r="L11" s="113"/>
+      <c r="M11" s="113"/>
+      <c r="N11" s="113"/>
+      <c r="O11" s="113"/>
+      <c r="P11" s="113"/>
+      <c r="Q11" s="113"/>
+      <c r="R11" s="113"/>
+      <c r="S11" s="112" t="s">
         <v>16</v>
       </c>
-      <c r="T11" s="67"/>
-      <c r="U11" s="67"/>
-      <c r="V11" s="67"/>
-      <c r="W11" s="72" t="s">
-        <v>23</v>
-      </c>
-      <c r="X11" s="72"/>
-      <c r="Y11" s="72"/>
-      <c r="Z11" s="72"/>
-      <c r="AA11" s="72"/>
-      <c r="AB11" s="72"/>
-      <c r="AC11" s="72"/>
-      <c r="AD11" s="72"/>
-      <c r="AE11" s="72"/>
-      <c r="AF11" s="73"/>
+      <c r="T11" s="112"/>
+      <c r="U11" s="112"/>
+      <c r="V11" s="112"/>
+      <c r="W11" s="117"/>
+      <c r="X11" s="117"/>
+      <c r="Y11" s="117"/>
+      <c r="Z11" s="117"/>
+      <c r="AA11" s="117"/>
+      <c r="AB11" s="117"/>
+      <c r="AC11" s="117"/>
+      <c r="AD11" s="117"/>
+      <c r="AE11" s="117"/>
+      <c r="AF11" s="118"/>
     </row>
     <row r="12" spans="1:32" ht="31.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65"/>
-      <c r="E12" s="74" t="s">
+      <c r="A12" s="108"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="109"/>
+      <c r="D12" s="110"/>
+      <c r="E12" s="119" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75"/>
-      <c r="H12" s="75"/>
-      <c r="I12" s="43" t="s">
-        <v>24</v>
-      </c>
-      <c r="J12" s="43"/>
-      <c r="K12" s="43"/>
-      <c r="L12" s="43"/>
-      <c r="M12" s="43"/>
-      <c r="N12" s="43"/>
-      <c r="O12" s="43"/>
-      <c r="P12" s="43"/>
-      <c r="Q12" s="43"/>
-      <c r="R12" s="43"/>
-      <c r="S12" s="75" t="s">
-        <v>25</v>
-      </c>
-      <c r="T12" s="75"/>
-      <c r="U12" s="75"/>
-      <c r="V12" s="75"/>
-      <c r="W12" s="76" t="s">
-        <v>26</v>
-      </c>
-      <c r="X12" s="77"/>
-      <c r="Y12" s="77"/>
-      <c r="Z12" s="77"/>
-      <c r="AA12" s="77"/>
-      <c r="AB12" s="77"/>
-      <c r="AC12" s="77"/>
-      <c r="AD12" s="77"/>
-      <c r="AE12" s="77"/>
-      <c r="AF12" s="78"/>
+      <c r="F12" s="120"/>
+      <c r="G12" s="120"/>
+      <c r="H12" s="120"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="86"/>
+      <c r="N12" s="86"/>
+      <c r="O12" s="86"/>
+      <c r="P12" s="86"/>
+      <c r="Q12" s="86"/>
+      <c r="R12" s="86"/>
+      <c r="S12" s="120" t="s">
+        <v>22</v>
+      </c>
+      <c r="T12" s="120"/>
+      <c r="U12" s="120"/>
+      <c r="V12" s="120"/>
+      <c r="W12" s="121"/>
+      <c r="X12" s="122"/>
+      <c r="Y12" s="122"/>
+      <c r="Z12" s="122"/>
+      <c r="AA12" s="122"/>
+      <c r="AB12" s="122"/>
+      <c r="AC12" s="122"/>
+      <c r="AD12" s="122"/>
+      <c r="AE12" s="122"/>
+      <c r="AF12" s="123"/>
     </row>
     <row r="14" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="89" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="89"/>
-      <c r="C14" s="89"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="89"/>
-      <c r="F14" s="89"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="89"/>
-      <c r="I14" s="89"/>
-      <c r="J14" s="89"/>
-      <c r="K14" s="89"/>
-      <c r="L14" s="89"/>
-      <c r="M14" s="89"/>
-      <c r="N14" s="89"/>
-      <c r="O14" s="89"/>
-      <c r="P14" s="89"/>
-      <c r="Q14" s="89"/>
-      <c r="R14" s="89"/>
-      <c r="S14" s="89"/>
-      <c r="T14" s="89"/>
-      <c r="U14" s="89"/>
-      <c r="V14" s="89"/>
-      <c r="W14" s="89"/>
-      <c r="X14" s="89"/>
-      <c r="Y14" s="89"/>
-      <c r="Z14" s="89"/>
-      <c r="AA14" s="89"/>
-      <c r="AB14" s="89"/>
-      <c r="AC14" s="89"/>
-      <c r="AD14" s="89"/>
-      <c r="AE14" s="89"/>
-      <c r="AF14" s="89"/>
+      <c r="A14" s="79" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" s="79"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="79"/>
+      <c r="E14" s="79"/>
+      <c r="F14" s="79"/>
+      <c r="G14" s="79"/>
+      <c r="H14" s="79"/>
+      <c r="I14" s="79"/>
+      <c r="J14" s="79"/>
+      <c r="K14" s="79"/>
+      <c r="L14" s="79"/>
+      <c r="M14" s="79"/>
+      <c r="N14" s="79"/>
+      <c r="O14" s="79"/>
+      <c r="P14" s="79"/>
+      <c r="Q14" s="79"/>
+      <c r="R14" s="79"/>
+      <c r="S14" s="79"/>
+      <c r="T14" s="79"/>
+      <c r="U14" s="79"/>
+      <c r="V14" s="79"/>
+      <c r="W14" s="79"/>
+      <c r="X14" s="79"/>
+      <c r="Y14" s="79"/>
+      <c r="Z14" s="79"/>
+      <c r="AA14" s="79"/>
+      <c r="AB14" s="79"/>
+      <c r="AC14" s="79"/>
+      <c r="AD14" s="79"/>
+      <c r="AE14" s="79"/>
+      <c r="AF14" s="79"/>
     </row>
     <row r="16" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="90" t="s">
-        <v>28</v>
-      </c>
-      <c r="B16" s="57"/>
-      <c r="C16" s="57"/>
-      <c r="D16" s="91"/>
-      <c r="E16" s="92">
-        <v>45666</v>
-      </c>
-      <c r="F16" s="57"/>
-      <c r="G16" s="57"/>
-      <c r="H16" s="57"/>
-      <c r="I16" s="57"/>
-      <c r="J16" s="57"/>
-      <c r="K16" s="57"/>
-      <c r="L16" s="57"/>
-      <c r="M16" s="57"/>
-      <c r="N16" s="57"/>
-      <c r="O16" s="57"/>
-      <c r="P16" s="57"/>
-      <c r="Q16" s="91" t="s">
-        <v>29</v>
-      </c>
-      <c r="R16" s="95"/>
-      <c r="S16" s="95"/>
-      <c r="T16" s="95"/>
-      <c r="U16" s="95"/>
-      <c r="V16" s="95"/>
-      <c r="W16" s="95"/>
-      <c r="X16" s="95"/>
-      <c r="Y16" s="95"/>
-      <c r="Z16" s="95"/>
-      <c r="AA16" s="95"/>
-      <c r="AB16" s="95"/>
-      <c r="AC16" s="95"/>
-      <c r="AD16" s="95"/>
-      <c r="AE16" s="95"/>
-      <c r="AF16" s="96"/>
+      <c r="A16" s="80" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="81"/>
+      <c r="C16" s="81"/>
+      <c r="D16" s="82"/>
+      <c r="E16" s="83"/>
+      <c r="F16" s="81"/>
+      <c r="G16" s="81"/>
+      <c r="H16" s="81"/>
+      <c r="I16" s="81"/>
+      <c r="J16" s="81"/>
+      <c r="K16" s="81"/>
+      <c r="L16" s="81"/>
+      <c r="M16" s="81"/>
+      <c r="N16" s="81"/>
+      <c r="O16" s="81"/>
+      <c r="P16" s="81"/>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="87"/>
+      <c r="S16" s="87"/>
+      <c r="T16" s="87"/>
+      <c r="U16" s="87"/>
+      <c r="V16" s="87"/>
+      <c r="W16" s="87"/>
+      <c r="X16" s="87"/>
+      <c r="Y16" s="87"/>
+      <c r="Z16" s="87"/>
+      <c r="AA16" s="87"/>
+      <c r="AB16" s="87"/>
+      <c r="AC16" s="87"/>
+      <c r="AD16" s="87"/>
+      <c r="AE16" s="87"/>
+      <c r="AF16" s="88"/>
     </row>
     <row r="17" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="86" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17" s="87"/>
-      <c r="C17" s="87"/>
-      <c r="D17" s="87"/>
-      <c r="E17" s="87" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="87"/>
-      <c r="G17" s="87"/>
-      <c r="H17" s="87"/>
-      <c r="I17" s="87"/>
-      <c r="J17" s="87"/>
-      <c r="K17" s="87"/>
-      <c r="L17" s="87"/>
-      <c r="M17" s="87"/>
-      <c r="N17" s="87"/>
-      <c r="O17" s="87"/>
-      <c r="P17" s="88"/>
-      <c r="Q17" s="97"/>
-      <c r="R17" s="87"/>
-      <c r="S17" s="87"/>
-      <c r="T17" s="87"/>
-      <c r="U17" s="87"/>
-      <c r="V17" s="87"/>
-      <c r="W17" s="87"/>
-      <c r="X17" s="87"/>
-      <c r="Y17" s="87"/>
-      <c r="Z17" s="87"/>
-      <c r="AA17" s="87"/>
-      <c r="AB17" s="87"/>
-      <c r="AC17" s="87"/>
-      <c r="AD17" s="87"/>
-      <c r="AE17" s="87"/>
-      <c r="AF17" s="98"/>
+      <c r="A17" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="77"/>
+      <c r="C17" s="77"/>
+      <c r="D17" s="77"/>
+      <c r="E17" s="77"/>
+      <c r="F17" s="77"/>
+      <c r="G17" s="77"/>
+      <c r="H17" s="77"/>
+      <c r="I17" s="77"/>
+      <c r="J17" s="77"/>
+      <c r="K17" s="77"/>
+      <c r="L17" s="77"/>
+      <c r="M17" s="77"/>
+      <c r="N17" s="77"/>
+      <c r="O17" s="77"/>
+      <c r="P17" s="78"/>
+      <c r="Q17" s="89"/>
+      <c r="R17" s="77"/>
+      <c r="S17" s="77"/>
+      <c r="T17" s="77"/>
+      <c r="U17" s="77"/>
+      <c r="V17" s="77"/>
+      <c r="W17" s="77"/>
+      <c r="X17" s="77"/>
+      <c r="Y17" s="77"/>
+      <c r="Z17" s="77"/>
+      <c r="AA17" s="77"/>
+      <c r="AB17" s="77"/>
+      <c r="AC17" s="77"/>
+      <c r="AD17" s="77"/>
+      <c r="AE17" s="77"/>
+      <c r="AF17" s="90"/>
     </row>
     <row r="18" spans="1:32" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="42" t="s">
+      <c r="A18" s="145" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="74"/>
+      <c r="E18" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="74"/>
+      <c r="G18" s="70"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="71"/>
+      <c r="J18" s="71"/>
+      <c r="K18" s="71"/>
+      <c r="L18" s="72"/>
+      <c r="M18" s="73" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="74"/>
+      <c r="O18" s="73" t="s">
+        <v>29</v>
+      </c>
+      <c r="P18" s="75"/>
+      <c r="Q18" s="85"/>
+      <c r="R18" s="85"/>
+      <c r="S18" s="85"/>
+      <c r="T18" s="85"/>
+      <c r="U18" s="85"/>
+      <c r="V18" s="85"/>
+      <c r="W18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="X18" s="73" t="s">
+        <v>31</v>
+      </c>
+      <c r="Y18" s="86"/>
+      <c r="Z18" s="74"/>
+      <c r="AA18" s="4"/>
+      <c r="AB18" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="45" t="s">
+      <c r="AC18" s="74"/>
+      <c r="AD18" s="5"/>
+      <c r="AE18" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="81" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="82"/>
-      <c r="I18" s="82"/>
-      <c r="J18" s="82"/>
-      <c r="K18" s="82"/>
-      <c r="L18" s="83"/>
-      <c r="M18" s="45" t="s">
-        <v>34</v>
-      </c>
-      <c r="N18" s="44"/>
-      <c r="O18" s="45" t="s">
-        <v>35</v>
-      </c>
-      <c r="P18" s="84"/>
-      <c r="Q18" s="94" t="s">
-        <v>36</v>
-      </c>
-      <c r="R18" s="94"/>
-      <c r="S18" s="94"/>
-      <c r="T18" s="94"/>
-      <c r="U18" s="94"/>
-      <c r="V18" s="94"/>
-      <c r="W18" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="X18" s="45" t="s">
-        <v>38</v>
-      </c>
-      <c r="Y18" s="43"/>
-      <c r="Z18" s="44"/>
-      <c r="AA18" s="4"/>
-      <c r="AB18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC18" s="44"/>
-      <c r="AD18" s="5"/>
-      <c r="AE18" s="79" t="s">
-        <v>40</v>
-      </c>
-      <c r="AF18" s="80"/>
+      <c r="AF18" s="69"/>
     </row>
     <row r="20" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="93" t="s">
+      <c r="A20" s="84" t="s">
+        <v>34</v>
+      </c>
+      <c r="B20" s="61"/>
+      <c r="C20" s="61" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="61"/>
+      <c r="E20" s="61"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="61"/>
+      <c r="H20" s="61" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="61"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="61" t="s">
+        <v>37</v>
+      </c>
+      <c r="L20" s="61"/>
+      <c r="M20" s="61"/>
+      <c r="N20" s="61" t="s">
+        <v>38</v>
+      </c>
+      <c r="O20" s="61"/>
+      <c r="P20" s="61"/>
+      <c r="Q20" s="61" t="s">
+        <v>39</v>
+      </c>
+      <c r="R20" s="61"/>
+      <c r="S20" s="61"/>
+      <c r="T20" s="61"/>
+      <c r="U20" s="61"/>
+      <c r="V20" s="61"/>
+      <c r="W20" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="X20" s="61"/>
+      <c r="Y20" s="61"/>
+      <c r="Z20" s="61"/>
+      <c r="AA20" s="61"/>
+      <c r="AB20" s="61"/>
+      <c r="AC20" s="61"/>
+      <c r="AD20" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="85"/>
-      <c r="C20" s="85" t="s">
-        <v>42</v>
-      </c>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85" t="s">
-        <v>43</v>
-      </c>
-      <c r="I20" s="85"/>
-      <c r="J20" s="85"/>
-      <c r="K20" s="85" t="s">
-        <v>44</v>
-      </c>
-      <c r="L20" s="85"/>
-      <c r="M20" s="85"/>
-      <c r="N20" s="85" t="s">
-        <v>45</v>
-      </c>
-      <c r="O20" s="85"/>
-      <c r="P20" s="85"/>
-      <c r="Q20" s="85" t="s">
-        <v>46</v>
-      </c>
-      <c r="R20" s="85"/>
-      <c r="S20" s="85"/>
-      <c r="T20" s="85"/>
-      <c r="U20" s="85"/>
-      <c r="V20" s="85"/>
-      <c r="W20" s="85" t="s">
-        <v>47</v>
-      </c>
-      <c r="X20" s="85"/>
-      <c r="Y20" s="85"/>
-      <c r="Z20" s="85"/>
-      <c r="AA20" s="85"/>
-      <c r="AB20" s="85"/>
-      <c r="AC20" s="85"/>
-      <c r="AD20" s="85" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE20" s="85"/>
-      <c r="AF20" s="107"/>
+      <c r="AE20" s="61"/>
+      <c r="AF20" s="65"/>
     </row>
     <row r="21" spans="1:32" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="99">
+      <c r="A21" s="54">
         <v>1</v>
       </c>
-      <c r="B21" s="18"/>
-      <c r="C21" s="19" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" s="100"/>
-      <c r="E21" s="100"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" s="100"/>
-      <c r="J21" s="101"/>
-      <c r="K21" s="19" t="s">
-        <v>51</v>
-      </c>
-      <c r="L21" s="100"/>
-      <c r="M21" s="101"/>
-      <c r="N21" s="19">
-        <v>1</v>
-      </c>
-      <c r="O21" s="100"/>
-      <c r="P21" s="101"/>
-      <c r="Q21" s="108">
-        <v>55000</v>
-      </c>
-      <c r="R21" s="104"/>
-      <c r="S21" s="104"/>
-      <c r="T21" s="104"/>
-      <c r="U21" s="104"/>
-      <c r="V21" s="109"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="36"/>
+      <c r="E21" s="36"/>
+      <c r="F21" s="36"/>
+      <c r="G21" s="30"/>
+      <c r="H21" s="25"/>
+      <c r="I21" s="36"/>
+      <c r="J21" s="30"/>
+      <c r="K21" s="25"/>
+      <c r="L21" s="36"/>
+      <c r="M21" s="30"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="36"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="66"/>
+      <c r="R21" s="64"/>
+      <c r="S21" s="64"/>
+      <c r="T21" s="64"/>
+      <c r="U21" s="64"/>
+      <c r="V21" s="67"/>
       <c r="W21" s="14"/>
-      <c r="X21" s="104">
-        <v>55000</v>
-      </c>
-      <c r="Y21" s="104"/>
-      <c r="Z21" s="104"/>
-      <c r="AA21" s="104"/>
-      <c r="AB21" s="104"/>
+      <c r="X21" s="64"/>
+      <c r="Y21" s="64"/>
+      <c r="Z21" s="64"/>
+      <c r="AA21" s="64"/>
+      <c r="AB21" s="64"/>
       <c r="AC21" s="6"/>
-      <c r="AD21" s="102"/>
-      <c r="AE21" s="102"/>
-      <c r="AF21" s="103"/>
+      <c r="AD21" s="62"/>
+      <c r="AE21" s="62"/>
+      <c r="AF21" s="63"/>
     </row>
     <row r="22" spans="1:32" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="99">
+      <c r="A22" s="54">
         <v>2</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D22" s="18"/>
-      <c r="E22" s="18"/>
-      <c r="F22" s="18"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="18"/>
-      <c r="J22" s="18"/>
-      <c r="K22" s="18" t="s">
-        <v>51</v>
-      </c>
-      <c r="L22" s="18"/>
-      <c r="M22" s="18"/>
-      <c r="N22" s="18">
-        <v>100</v>
-      </c>
-      <c r="O22" s="18"/>
-      <c r="P22" s="18"/>
-      <c r="Q22" s="108">
-        <v>19580</v>
-      </c>
-      <c r="R22" s="105"/>
-      <c r="S22" s="105"/>
-      <c r="T22" s="105"/>
-      <c r="U22" s="105"/>
-      <c r="V22" s="110"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="66"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="31"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="32"/>
       <c r="W22" s="14"/>
-      <c r="X22" s="104">
-        <v>1958000</v>
-      </c>
-      <c r="Y22" s="105"/>
-      <c r="Z22" s="105"/>
-      <c r="AA22" s="105"/>
-      <c r="AB22" s="105"/>
+      <c r="X22" s="64"/>
+      <c r="Y22" s="31"/>
+      <c r="Z22" s="31"/>
+      <c r="AA22" s="31"/>
+      <c r="AB22" s="31"/>
       <c r="AC22" s="6"/>
-      <c r="AD22" s="18"/>
-      <c r="AE22" s="18"/>
-      <c r="AF22" s="106"/>
+      <c r="AD22" s="21"/>
+      <c r="AE22" s="21"/>
+      <c r="AF22" s="38"/>
     </row>
     <row r="23" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="99">
+      <c r="A23" s="54">
         <v>3</v>
       </c>
-      <c r="B23" s="18"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
-      <c r="M23" s="18"/>
-      <c r="N23" s="18"/>
-      <c r="O23" s="18"/>
-      <c r="P23" s="18"/>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="16"/>
-      <c r="S23" s="17"/>
-      <c r="T23" s="18"/>
-      <c r="U23" s="19"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="23"/>
+      <c r="S23" s="24"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="25"/>
       <c r="V23" s="6"/>
-      <c r="W23" s="15"/>
-      <c r="X23" s="16"/>
-      <c r="Y23" s="116"/>
-      <c r="Z23" s="117"/>
-      <c r="AA23" s="117"/>
-      <c r="AB23" s="118"/>
+      <c r="W23" s="22"/>
+      <c r="X23" s="23"/>
+      <c r="Y23" s="26"/>
+      <c r="Z23" s="27"/>
+      <c r="AA23" s="27"/>
+      <c r="AB23" s="28"/>
       <c r="AC23" s="6"/>
-      <c r="AD23" s="18"/>
-      <c r="AE23" s="18"/>
-      <c r="AF23" s="106"/>
+      <c r="AD23" s="21"/>
+      <c r="AE23" s="21"/>
+      <c r="AF23" s="38"/>
     </row>
     <row r="24" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="127">
+      <c r="A24" s="29">
         <v>4</v>
       </c>
-      <c r="B24" s="101"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="18"/>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18"/>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18"/>
-      <c r="O24" s="18"/>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="17"/>
-      <c r="T24" s="18"/>
-      <c r="U24" s="19"/>
+      <c r="B24" s="30"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="23"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="21"/>
+      <c r="U24" s="25"/>
       <c r="V24" s="6"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="116"/>
-      <c r="Z24" s="117"/>
-      <c r="AA24" s="117"/>
-      <c r="AB24" s="118"/>
+      <c r="W24" s="22"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="26"/>
+      <c r="Z24" s="27"/>
+      <c r="AA24" s="27"/>
+      <c r="AB24" s="28"/>
       <c r="AC24" s="6"/>
-      <c r="AD24" s="18"/>
-      <c r="AE24" s="18"/>
-      <c r="AF24" s="106"/>
+      <c r="AD24" s="21"/>
+      <c r="AE24" s="21"/>
+      <c r="AF24" s="38"/>
     </row>
     <row r="25" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="127">
+      <c r="A25" s="29">
         <v>5</v>
       </c>
-      <c r="B25" s="101"/>
-      <c r="C25" s="18"/>
-      <c r="D25" s="18"/>
-      <c r="E25" s="18"/>
-      <c r="F25" s="18"/>
-      <c r="G25" s="18"/>
-      <c r="H25" s="18"/>
-      <c r="I25" s="18"/>
-      <c r="J25" s="18"/>
-      <c r="K25" s="18"/>
-      <c r="L25" s="18"/>
-      <c r="M25" s="18"/>
-      <c r="N25" s="18"/>
-      <c r="O25" s="18"/>
-      <c r="P25" s="18"/>
-      <c r="Q25" s="16"/>
-      <c r="R25" s="105"/>
-      <c r="S25" s="105"/>
-      <c r="T25" s="105"/>
-      <c r="U25" s="105"/>
-      <c r="V25" s="110"/>
-      <c r="W25" s="16"/>
-      <c r="X25" s="105"/>
-      <c r="Y25" s="105"/>
-      <c r="Z25" s="105"/>
-      <c r="AA25" s="105"/>
-      <c r="AB25" s="105"/>
-      <c r="AC25" s="110"/>
-      <c r="AD25" s="19"/>
-      <c r="AE25" s="100"/>
-      <c r="AF25" s="135"/>
+      <c r="B25" s="30"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="23"/>
+      <c r="R25" s="31"/>
+      <c r="S25" s="31"/>
+      <c r="T25" s="31"/>
+      <c r="U25" s="31"/>
+      <c r="V25" s="32"/>
+      <c r="W25" s="23"/>
+      <c r="X25" s="31"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="31"/>
+      <c r="AC25" s="32"/>
+      <c r="AD25" s="25"/>
+      <c r="AE25" s="36"/>
+      <c r="AF25" s="37"/>
     </row>
     <row r="26" spans="1:32" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="99">
+      <c r="A26" s="54">
         <v>6</v>
       </c>
-      <c r="B26" s="18"/>
-      <c r="C26" s="18"/>
-      <c r="D26" s="18"/>
-      <c r="E26" s="18"/>
-      <c r="F26" s="18"/>
-      <c r="G26" s="18"/>
-      <c r="H26" s="18"/>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="15"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="17"/>
-      <c r="T26" s="18"/>
-      <c r="U26" s="19"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="23"/>
+      <c r="S26" s="24"/>
+      <c r="T26" s="21"/>
+      <c r="U26" s="25"/>
       <c r="V26" s="6"/>
-      <c r="W26" s="15"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="116"/>
-      <c r="Z26" s="117"/>
-      <c r="AA26" s="117"/>
-      <c r="AB26" s="118"/>
+      <c r="W26" s="22"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="26"/>
+      <c r="Z26" s="27"/>
+      <c r="AA26" s="27"/>
+      <c r="AB26" s="28"/>
       <c r="AC26" s="6"/>
-      <c r="AD26" s="18"/>
-      <c r="AE26" s="18"/>
-      <c r="AF26" s="106"/>
+      <c r="AD26" s="21"/>
+      <c r="AE26" s="21"/>
+      <c r="AF26" s="38"/>
     </row>
     <row r="27" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="124" t="s">
-        <v>53</v>
-      </c>
-      <c r="B27" s="125"/>
-      <c r="C27" s="125"/>
-      <c r="D27" s="125"/>
-      <c r="E27" s="125"/>
-      <c r="F27" s="125"/>
-      <c r="G27" s="125"/>
-      <c r="H27" s="125"/>
-      <c r="I27" s="125"/>
-      <c r="J27" s="125"/>
-      <c r="K27" s="125"/>
-      <c r="L27" s="125"/>
-      <c r="M27" s="126"/>
-      <c r="N27" s="119">
+      <c r="A27" s="58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="60"/>
+      <c r="N27" s="55">
         <f>SUM(N21:P26)</f>
-        <v>101</v>
-      </c>
-      <c r="O27" s="120"/>
-      <c r="P27" s="121"/>
-      <c r="Q27" s="134">
+        <v>0</v>
+      </c>
+      <c r="O27" s="34"/>
+      <c r="P27" s="35"/>
+      <c r="Q27" s="33">
         <f>SUM(Q21:V26)</f>
-        <v>74580</v>
-      </c>
-      <c r="R27" s="120"/>
-      <c r="S27" s="120"/>
-      <c r="T27" s="120"/>
-      <c r="U27" s="120"/>
-      <c r="V27" s="121"/>
-      <c r="W27" s="134">
+        <v>0</v>
+      </c>
+      <c r="R27" s="34"/>
+      <c r="S27" s="34"/>
+      <c r="T27" s="34"/>
+      <c r="U27" s="34"/>
+      <c r="V27" s="35"/>
+      <c r="W27" s="33">
         <f>SUM(W21:AC26)</f>
-        <v>2013000</v>
-      </c>
-      <c r="X27" s="120"/>
-      <c r="Y27" s="120"/>
-      <c r="Z27" s="120"/>
-      <c r="AA27" s="120"/>
-      <c r="AB27" s="121"/>
+        <v>0</v>
+      </c>
+      <c r="X27" s="34"/>
+      <c r="Y27" s="34"/>
+      <c r="Z27" s="34"/>
+      <c r="AA27" s="34"/>
+      <c r="AB27" s="35"/>
       <c r="AC27" s="7"/>
-      <c r="AD27" s="122"/>
-      <c r="AE27" s="122"/>
-      <c r="AF27" s="123"/>
+      <c r="AD27" s="56"/>
+      <c r="AE27" s="56"/>
+      <c r="AF27" s="57"/>
     </row>
     <row r="28" spans="1:32" ht="12" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="29" spans="1:32" ht="20" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="136" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="137"/>
-      <c r="C29" s="137"/>
-      <c r="D29" s="137"/>
-      <c r="E29" s="137"/>
-      <c r="F29" s="137"/>
-      <c r="G29" s="137"/>
-      <c r="H29" s="137"/>
-      <c r="I29" s="137"/>
-      <c r="J29" s="137"/>
-      <c r="K29" s="137"/>
-      <c r="L29" s="137"/>
-      <c r="M29" s="137"/>
-      <c r="N29" s="137"/>
-      <c r="O29" s="137"/>
-      <c r="P29" s="137"/>
-      <c r="Q29" s="137"/>
-      <c r="R29" s="137"/>
-      <c r="S29" s="137"/>
-      <c r="T29" s="137"/>
-      <c r="U29" s="137"/>
-      <c r="V29" s="137"/>
-      <c r="W29" s="137"/>
-      <c r="X29" s="137"/>
-      <c r="Y29" s="137"/>
-      <c r="Z29" s="137"/>
-      <c r="AA29" s="137"/>
-      <c r="AB29" s="137"/>
-      <c r="AC29" s="137"/>
-      <c r="AD29" s="137"/>
-      <c r="AE29" s="137"/>
-      <c r="AF29" s="138"/>
+      <c r="A29" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B29" s="40"/>
+      <c r="C29" s="40"/>
+      <c r="D29" s="40"/>
+      <c r="E29" s="40"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="40"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
+      <c r="K29" s="40"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="40"/>
+      <c r="N29" s="40"/>
+      <c r="O29" s="40"/>
+      <c r="P29" s="40"/>
+      <c r="Q29" s="40"/>
+      <c r="R29" s="40"/>
+      <c r="S29" s="40"/>
+      <c r="T29" s="40"/>
+      <c r="U29" s="40"/>
+      <c r="V29" s="40"/>
+      <c r="W29" s="40"/>
+      <c r="X29" s="40"/>
+      <c r="Y29" s="40"/>
+      <c r="Z29" s="40"/>
+      <c r="AA29" s="40"/>
+      <c r="AB29" s="40"/>
+      <c r="AC29" s="40"/>
+      <c r="AD29" s="40"/>
+      <c r="AE29" s="40"/>
+      <c r="AF29" s="41"/>
     </row>
     <row r="30" spans="1:32" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="142"/>
-      <c r="B30" s="143"/>
-      <c r="C30" s="143"/>
-      <c r="D30" s="143"/>
-      <c r="E30" s="143"/>
-      <c r="F30" s="143"/>
-      <c r="G30" s="143"/>
-      <c r="H30" s="143"/>
-      <c r="I30" s="143"/>
-      <c r="J30" s="143"/>
-      <c r="K30" s="143"/>
-      <c r="L30" s="143"/>
-      <c r="M30" s="143"/>
-      <c r="N30" s="143"/>
-      <c r="O30" s="143"/>
-      <c r="P30" s="143"/>
-      <c r="Q30" s="143"/>
-      <c r="R30" s="143"/>
-      <c r="S30" s="143"/>
-      <c r="T30" s="143"/>
-      <c r="U30" s="143"/>
-      <c r="V30" s="143"/>
+      <c r="A30" s="45"/>
+      <c r="B30" s="46"/>
+      <c r="C30" s="46"/>
+      <c r="D30" s="46"/>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
+      <c r="J30" s="46"/>
+      <c r="K30" s="46"/>
+      <c r="L30" s="46"/>
+      <c r="M30" s="46"/>
+      <c r="N30" s="46"/>
+      <c r="O30" s="46"/>
+      <c r="P30" s="46"/>
+      <c r="Q30" s="46"/>
+      <c r="R30" s="46"/>
+      <c r="S30" s="46"/>
+      <c r="T30" s="46"/>
+      <c r="U30" s="46"/>
+      <c r="V30" s="46"/>
       <c r="W30" s="9"/>
       <c r="X30" s="9"/>
       <c r="Y30" s="9"/>
@@ -3184,153 +3088,258 @@
       <c r="AF30" s="10"/>
     </row>
     <row r="31" spans="1:32" ht="26" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="144"/>
-      <c r="B31" s="145"/>
-      <c r="C31" s="145"/>
-      <c r="D31" s="145"/>
-      <c r="E31" s="145"/>
-      <c r="F31" s="145"/>
-      <c r="G31" s="145"/>
-      <c r="H31" s="145"/>
-      <c r="I31" s="145"/>
-      <c r="J31" s="145"/>
-      <c r="K31" s="145"/>
-      <c r="L31" s="145"/>
-      <c r="M31" s="145"/>
-      <c r="N31" s="145"/>
-      <c r="O31" s="145"/>
-      <c r="P31" s="145"/>
-      <c r="Q31" s="145"/>
-      <c r="R31" s="145"/>
-      <c r="S31" s="145"/>
-      <c r="T31" s="145"/>
-      <c r="U31" s="145"/>
-      <c r="V31" s="145"/>
-      <c r="W31" s="115" t="s">
-        <v>55</v>
-      </c>
-      <c r="X31" s="115"/>
-      <c r="Y31" s="115"/>
+      <c r="A31" s="47"/>
+      <c r="B31" s="48"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="H31" s="48"/>
+      <c r="I31" s="48"/>
+      <c r="J31" s="48"/>
+      <c r="K31" s="48"/>
+      <c r="L31" s="48"/>
+      <c r="M31" s="48"/>
+      <c r="N31" s="48"/>
+      <c r="O31" s="48"/>
+      <c r="P31" s="48"/>
+      <c r="Q31" s="48"/>
+      <c r="R31" s="48"/>
+      <c r="S31" s="48"/>
+      <c r="T31" s="48"/>
+      <c r="U31" s="48"/>
+      <c r="V31" s="48"/>
+      <c r="W31" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="X31" s="53"/>
+      <c r="Y31" s="53"/>
       <c r="Z31" s="12"/>
-      <c r="AA31" s="111" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB31" s="112"/>
+      <c r="AA31" s="49" t="s">
+        <v>45</v>
+      </c>
+      <c r="AB31" s="50"/>
       <c r="AC31" s="13"/>
-      <c r="AD31" s="113" t="s">
-        <v>57</v>
-      </c>
-      <c r="AE31" s="114"/>
+      <c r="AD31" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="AE31" s="52"/>
       <c r="AF31" s="11"/>
     </row>
     <row r="32" spans="1:32" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="139" t="s">
-        <v>58</v>
-      </c>
-      <c r="B32" s="140"/>
-      <c r="C32" s="140"/>
-      <c r="D32" s="140"/>
-      <c r="E32" s="140"/>
-      <c r="F32" s="140"/>
-      <c r="G32" s="140"/>
-      <c r="H32" s="140"/>
-      <c r="I32" s="140"/>
-      <c r="J32" s="140"/>
-      <c r="K32" s="140"/>
-      <c r="L32" s="140"/>
-      <c r="M32" s="140"/>
-      <c r="N32" s="140"/>
-      <c r="O32" s="140"/>
-      <c r="P32" s="140"/>
-      <c r="Q32" s="140"/>
-      <c r="R32" s="140"/>
-      <c r="S32" s="140"/>
-      <c r="T32" s="140"/>
-      <c r="U32" s="140"/>
-      <c r="V32" s="140"/>
-      <c r="W32" s="140"/>
-      <c r="X32" s="140"/>
-      <c r="Y32" s="140"/>
-      <c r="Z32" s="140"/>
-      <c r="AA32" s="140"/>
-      <c r="AB32" s="140"/>
-      <c r="AC32" s="140"/>
-      <c r="AD32" s="140"/>
-      <c r="AE32" s="140"/>
-      <c r="AF32" s="141"/>
+      <c r="A32" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="43"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="43"/>
+      <c r="O32" s="43"/>
+      <c r="P32" s="43"/>
+      <c r="Q32" s="43"/>
+      <c r="R32" s="43"/>
+      <c r="S32" s="43"/>
+      <c r="T32" s="43"/>
+      <c r="U32" s="43"/>
+      <c r="V32" s="43"/>
+      <c r="W32" s="43"/>
+      <c r="X32" s="43"/>
+      <c r="Y32" s="43"/>
+      <c r="Z32" s="43"/>
+      <c r="AA32" s="43"/>
+      <c r="AB32" s="43"/>
+      <c r="AC32" s="43"/>
+      <c r="AD32" s="43"/>
+      <c r="AE32" s="43"/>
+      <c r="AF32" s="44"/>
     </row>
     <row r="33" spans="1:32" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="128" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" s="129"/>
-      <c r="C33" s="129"/>
-      <c r="D33" s="129"/>
-      <c r="E33" s="129"/>
-      <c r="F33" s="129"/>
-      <c r="G33" s="129"/>
-      <c r="H33" s="129"/>
-      <c r="I33" s="129"/>
-      <c r="J33" s="129"/>
-      <c r="K33" s="129"/>
-      <c r="L33" s="129"/>
-      <c r="M33" s="129"/>
-      <c r="N33" s="129"/>
-      <c r="O33" s="129"/>
-      <c r="P33" s="129"/>
-      <c r="Q33" s="129"/>
-      <c r="R33" s="129"/>
-      <c r="S33" s="129"/>
-      <c r="T33" s="129"/>
-      <c r="U33" s="129"/>
-      <c r="V33" s="129"/>
-      <c r="W33" s="129"/>
-      <c r="X33" s="129"/>
-      <c r="Y33" s="129"/>
-      <c r="Z33" s="129"/>
-      <c r="AA33" s="129"/>
-      <c r="AB33" s="129"/>
-      <c r="AC33" s="129"/>
-      <c r="AD33" s="129"/>
-      <c r="AE33" s="129"/>
-      <c r="AF33" s="130"/>
+      <c r="A33" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
+      <c r="D33" s="16"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="16"/>
+      <c r="H33" s="16"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="16"/>
+      <c r="K33" s="16"/>
+      <c r="L33" s="16"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="16"/>
+      <c r="O33" s="16"/>
+      <c r="P33" s="16"/>
+      <c r="Q33" s="16"/>
+      <c r="R33" s="16"/>
+      <c r="S33" s="16"/>
+      <c r="T33" s="16"/>
+      <c r="U33" s="16"/>
+      <c r="V33" s="16"/>
+      <c r="W33" s="16"/>
+      <c r="X33" s="16"/>
+      <c r="Y33" s="16"/>
+      <c r="Z33" s="16"/>
+      <c r="AA33" s="16"/>
+      <c r="AB33" s="16"/>
+      <c r="AC33" s="16"/>
+      <c r="AD33" s="16"/>
+      <c r="AE33" s="16"/>
+      <c r="AF33" s="17"/>
     </row>
     <row r="34" spans="1:32" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="131"/>
-      <c r="B34" s="132"/>
-      <c r="C34" s="132"/>
-      <c r="D34" s="132"/>
-      <c r="E34" s="132"/>
-      <c r="F34" s="132"/>
-      <c r="G34" s="132"/>
-      <c r="H34" s="132"/>
-      <c r="I34" s="132"/>
-      <c r="J34" s="132"/>
-      <c r="K34" s="132"/>
-      <c r="L34" s="132"/>
-      <c r="M34" s="132"/>
-      <c r="N34" s="132"/>
-      <c r="O34" s="132"/>
-      <c r="P34" s="132"/>
-      <c r="Q34" s="132"/>
-      <c r="R34" s="132"/>
-      <c r="S34" s="132"/>
-      <c r="T34" s="132"/>
-      <c r="U34" s="132"/>
-      <c r="V34" s="132"/>
-      <c r="W34" s="132"/>
-      <c r="X34" s="132"/>
-      <c r="Y34" s="132"/>
-      <c r="Z34" s="132"/>
-      <c r="AA34" s="132"/>
-      <c r="AB34" s="132"/>
-      <c r="AC34" s="132"/>
-      <c r="AD34" s="132"/>
-      <c r="AE34" s="132"/>
-      <c r="AF34" s="133"/>
+      <c r="A34" s="18"/>
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="19"/>
+      <c r="E34" s="19"/>
+      <c r="F34" s="19"/>
+      <c r="G34" s="19"/>
+      <c r="H34" s="19"/>
+      <c r="I34" s="19"/>
+      <c r="J34" s="19"/>
+      <c r="K34" s="19"/>
+      <c r="L34" s="19"/>
+      <c r="M34" s="19"/>
+      <c r="N34" s="19"/>
+      <c r="O34" s="19"/>
+      <c r="P34" s="19"/>
+      <c r="Q34" s="19"/>
+      <c r="R34" s="19"/>
+      <c r="S34" s="19"/>
+      <c r="T34" s="19"/>
+      <c r="U34" s="19"/>
+      <c r="V34" s="19"/>
+      <c r="W34" s="19"/>
+      <c r="X34" s="19"/>
+      <c r="Y34" s="19"/>
+      <c r="Z34" s="19"/>
+      <c r="AA34" s="19"/>
+      <c r="AB34" s="19"/>
+      <c r="AC34" s="19"/>
+      <c r="AD34" s="19"/>
+      <c r="AE34" s="19"/>
+      <c r="AF34" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="129">
+    <mergeCell ref="Q24:R24"/>
+    <mergeCell ref="S24:U24"/>
+    <mergeCell ref="K2:O3"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="Q4:T4"/>
+    <mergeCell ref="Q5:T5"/>
+    <mergeCell ref="Q2:T2"/>
+    <mergeCell ref="U2:AF2"/>
+    <mergeCell ref="Q3:T3"/>
+    <mergeCell ref="U3:AF3"/>
+    <mergeCell ref="U4:AF4"/>
+    <mergeCell ref="A5:D5"/>
+    <mergeCell ref="E5:I5"/>
+    <mergeCell ref="U5:AF5"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="I2:J3"/>
+    <mergeCell ref="A6:O7"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="U6:AF6"/>
+    <mergeCell ref="Q7:T7"/>
+    <mergeCell ref="U7:Y7"/>
+    <mergeCell ref="Z7:AA7"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="AB7:AF7"/>
+    <mergeCell ref="W10:AF10"/>
+    <mergeCell ref="A9:D10"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="I9:R9"/>
+    <mergeCell ref="S9:V9"/>
+    <mergeCell ref="W9:AF9"/>
+    <mergeCell ref="A11:D12"/>
+    <mergeCell ref="E11:H11"/>
+    <mergeCell ref="I11:R11"/>
+    <mergeCell ref="S11:V11"/>
+    <mergeCell ref="E10:H10"/>
+    <mergeCell ref="I10:R10"/>
+    <mergeCell ref="S10:V10"/>
+    <mergeCell ref="W11:AF11"/>
+    <mergeCell ref="E12:H12"/>
+    <mergeCell ref="I12:R12"/>
+    <mergeCell ref="S12:V12"/>
+    <mergeCell ref="W12:AF12"/>
+    <mergeCell ref="AE18:AF18"/>
+    <mergeCell ref="G18:L18"/>
+    <mergeCell ref="M18:N18"/>
+    <mergeCell ref="O18:P18"/>
+    <mergeCell ref="N20:P20"/>
+    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="E17:P17"/>
+    <mergeCell ref="A14:AF14"/>
+    <mergeCell ref="A16:D16"/>
+    <mergeCell ref="E16:P16"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="AB18:AC18"/>
+    <mergeCell ref="Q18:V18"/>
+    <mergeCell ref="X18:Z18"/>
+    <mergeCell ref="Q16:AF16"/>
+    <mergeCell ref="Q17:AF17"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="C20:G20"/>
+    <mergeCell ref="C21:G21"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="AD21:AF21"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="C22:G22"/>
+    <mergeCell ref="H22:J22"/>
+    <mergeCell ref="K22:M22"/>
+    <mergeCell ref="N22:P22"/>
+    <mergeCell ref="X21:AB21"/>
+    <mergeCell ref="X22:AB22"/>
+    <mergeCell ref="AD22:AF22"/>
+    <mergeCell ref="W20:AC20"/>
+    <mergeCell ref="AD20:AF20"/>
+    <mergeCell ref="Q21:V21"/>
+    <mergeCell ref="Q22:V22"/>
+    <mergeCell ref="H21:J21"/>
+    <mergeCell ref="K20:M20"/>
+    <mergeCell ref="K21:M21"/>
+    <mergeCell ref="N21:P21"/>
+    <mergeCell ref="Q20:V20"/>
+    <mergeCell ref="AA31:AB31"/>
+    <mergeCell ref="AD31:AE31"/>
+    <mergeCell ref="W31:Y31"/>
+    <mergeCell ref="Y26:AB26"/>
+    <mergeCell ref="AD26:AF26"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="C23:G23"/>
+    <mergeCell ref="N27:P27"/>
+    <mergeCell ref="AD27:AF27"/>
+    <mergeCell ref="A27:M27"/>
+    <mergeCell ref="W24:X24"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="C26:G26"/>
+    <mergeCell ref="H26:J26"/>
+    <mergeCell ref="K26:M26"/>
+    <mergeCell ref="N26:P26"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="Y24:AB24"/>
+    <mergeCell ref="AD24:AF24"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="C24:G24"/>
+    <mergeCell ref="H24:J24"/>
+    <mergeCell ref="K24:M24"/>
+    <mergeCell ref="N24:P24"/>
     <mergeCell ref="A33:AF34"/>
     <mergeCell ref="H23:J23"/>
     <mergeCell ref="K23:M23"/>
@@ -3355,129 +3364,23 @@
     <mergeCell ref="A29:AF29"/>
     <mergeCell ref="A32:AF32"/>
     <mergeCell ref="A30:V31"/>
-    <mergeCell ref="AA31:AB31"/>
-    <mergeCell ref="AD31:AE31"/>
-    <mergeCell ref="W31:Y31"/>
-    <mergeCell ref="Y26:AB26"/>
-    <mergeCell ref="AD26:AF26"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="C23:G23"/>
-    <mergeCell ref="N27:P27"/>
-    <mergeCell ref="AD27:AF27"/>
-    <mergeCell ref="A27:M27"/>
-    <mergeCell ref="W24:X24"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="C26:G26"/>
-    <mergeCell ref="H26:J26"/>
-    <mergeCell ref="K26:M26"/>
-    <mergeCell ref="N26:P26"/>
-    <mergeCell ref="Q26:R26"/>
-    <mergeCell ref="Y24:AB24"/>
-    <mergeCell ref="AD24:AF24"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="C24:G24"/>
-    <mergeCell ref="H24:J24"/>
-    <mergeCell ref="K24:M24"/>
-    <mergeCell ref="N24:P24"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="C20:G20"/>
-    <mergeCell ref="C21:G21"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="AD21:AF21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="C22:G22"/>
-    <mergeCell ref="H22:J22"/>
-    <mergeCell ref="K22:M22"/>
-    <mergeCell ref="N22:P22"/>
-    <mergeCell ref="X21:AB21"/>
-    <mergeCell ref="X22:AB22"/>
-    <mergeCell ref="AD22:AF22"/>
-    <mergeCell ref="W20:AC20"/>
-    <mergeCell ref="AD20:AF20"/>
-    <mergeCell ref="Q21:V21"/>
-    <mergeCell ref="Q22:V22"/>
-    <mergeCell ref="H21:J21"/>
-    <mergeCell ref="K20:M20"/>
-    <mergeCell ref="K21:M21"/>
-    <mergeCell ref="N21:P21"/>
-    <mergeCell ref="Q20:V20"/>
-    <mergeCell ref="AE18:AF18"/>
-    <mergeCell ref="G18:L18"/>
-    <mergeCell ref="M18:N18"/>
-    <mergeCell ref="O18:P18"/>
-    <mergeCell ref="N20:P20"/>
-    <mergeCell ref="A17:D17"/>
-    <mergeCell ref="E17:P17"/>
-    <mergeCell ref="A14:AF14"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="E16:P16"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="AB18:AC18"/>
-    <mergeCell ref="Q18:V18"/>
-    <mergeCell ref="X18:Z18"/>
-    <mergeCell ref="Q16:AF16"/>
-    <mergeCell ref="Q17:AF17"/>
-    <mergeCell ref="AB7:AF7"/>
-    <mergeCell ref="W10:AF10"/>
-    <mergeCell ref="A9:D10"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="I9:R9"/>
-    <mergeCell ref="S9:V9"/>
-    <mergeCell ref="W9:AF9"/>
-    <mergeCell ref="A11:D12"/>
-    <mergeCell ref="E11:H11"/>
-    <mergeCell ref="I11:R11"/>
-    <mergeCell ref="S11:V11"/>
-    <mergeCell ref="E10:H10"/>
-    <mergeCell ref="I10:R10"/>
-    <mergeCell ref="S10:V10"/>
-    <mergeCell ref="W11:AF11"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="I12:R12"/>
-    <mergeCell ref="S12:V12"/>
-    <mergeCell ref="W12:AF12"/>
-    <mergeCell ref="Q24:R24"/>
-    <mergeCell ref="S24:U24"/>
-    <mergeCell ref="K2:O3"/>
-    <mergeCell ref="D2:H3"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="Q5:T5"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="U2:AF2"/>
-    <mergeCell ref="Q3:T3"/>
-    <mergeCell ref="U3:AF3"/>
-    <mergeCell ref="U4:AF4"/>
-    <mergeCell ref="A5:D5"/>
-    <mergeCell ref="E5:I5"/>
-    <mergeCell ref="U5:AF5"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="I2:J3"/>
-    <mergeCell ref="A6:O7"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="U6:AF6"/>
-    <mergeCell ref="Q7:T7"/>
-    <mergeCell ref="U7:Y7"/>
-    <mergeCell ref="Z7:AA7"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E18:F18"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="U6" r:id="rId1" xr:uid="{B6137B18-27A7-3B4D-81C2-437325706A61}"/>
-    <hyperlink ref="W12" r:id="rId2" xr:uid="{FDBE7BEE-45E8-485C-B3BA-64FB58A6ED13}"/>
   </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.70866141732283505" right="0.70866141732283505" top="0.44" bottom="0.36" header="0.25" footer="0.17"/>
   <pageSetup paperSize="9" scale="92" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
-  <drawing r:id="rId3"/>
-  <legacyDrawing r:id="rId4"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x14">
       <controls>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1032" r:id="rId5" name="Check Box 8">
+            <control shapeId="1032" r:id="rId4" name="Check Box 8">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3499,7 +3402,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1033" r:id="rId6" name="Check Box 9">
+            <control shapeId="1033" r:id="rId5" name="Check Box 9">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3521,7 +3424,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1034" r:id="rId7" name="Check Box 10">
+            <control shapeId="1034" r:id="rId6" name="Check Box 10">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -3543,7 +3446,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1035" r:id="rId8" name="Check Box 11">
+            <control shapeId="1035" r:id="rId7" name="Check Box 11">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>